<commit_message>
Use single plot function!
</commit_message>
<xml_diff>
--- a/Code/Python/Experiments/Light_experiment_11-10_and_23-11.xlsx
+++ b/Code/Python/Experiments/Light_experiment_11-10_and_23-11.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
   <si>
     <t xml:space="preserve">Lamp 60 W halogeen</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t xml:space="preserve">Digikey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.85</t>
   </si>
   <si>
     <t xml:space="preserve">Nuon Solar</t>
@@ -213,11 +210,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,11 +592,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,10 +1131,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,16 +1463,16 @@
   <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.515306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,14 +1525,14 @@
       <c r="A4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>16</v>
+      <c r="B4" s="0" t="n">
+        <v>3.85</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3966</v>
+        <v>3.966</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>3731</v>
+        <v>3.731</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>4.031</v>
@@ -1548,7 +1543,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1.369</v>
@@ -1568,27 +1563,27 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>43062</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update python and excel files!
</commit_message>
<xml_diff>
--- a/Code/Python/Experiments/Light_experiment_11-10_and_23-11.xlsx
+++ b/Code/Python/Experiments/Light_experiment_11-10_and_23-11.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
     <t xml:space="preserve">Lamp 60 W halogeen</t>
   </si>
@@ -58,10 +58,16 @@
     <t xml:space="preserve">OLD</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">n</t>
   </si>
   <si>
     <t xml:space="preserve">Solar panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVG</t>
   </si>
   <si>
     <t xml:space="preserve">Chineese</t>
@@ -202,17 +208,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.7142857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.5357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -233,12 +242,6 @@
       <c r="D2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -254,10 +257,14 @@
         <v>26.08</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>577</v>
+        <f aca="false">AVERAGE(B3:D3)</f>
+        <v>26.2766666666667</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -274,10 +281,14 @@
         <v>6.481</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>2460</v>
+        <f aca="false">AVERAGE(B4:D4)</f>
+        <v>6.453</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>23</v>
+        <v>577</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -294,10 +305,14 @@
         <v>3.124</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>5790</v>
+        <f aca="false">AVERAGE(B5:D5)</f>
+        <v>3.08366666666667</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>25</v>
+        <v>2460</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -314,9 +329,21 @@
         <v>1.356</v>
       </c>
       <c r="E6" s="0" t="n">
+        <f aca="false">AVERAGE(B6:D6)</f>
+        <v>1.34833333333333</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>5790</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="0" t="n">
         <v>9550</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>42</v>
       </c>
     </row>
@@ -353,10 +380,8 @@
         <v>17.64</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1179</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>23</v>
+        <f aca="false">AVERAGE(B10:D10)</f>
+        <v>17.5936666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,10 +398,14 @@
         <v>6.694</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>2496</v>
+        <f aca="false">AVERAGE(B11:D11)</f>
+        <v>6.721</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>25</v>
+        <v>1179</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,9 +422,21 @@
         <v>2.706</v>
       </c>
       <c r="E12" s="0" t="n">
+        <f aca="false">AVERAGE(B12:D12)</f>
+        <v>2.19266666666667</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>2496</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="0" t="n">
         <v>8760</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="G13" s="0" t="n">
         <v>35</v>
       </c>
     </row>
@@ -417,9 +458,6 @@
       <c r="D15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -435,10 +473,11 @@
         <v>18.15</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>1027</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>26</v>
+        <f aca="false">AVERAGE(B16:D16)</f>
+        <v>17.9133333333333</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,10 +494,14 @@
         <v>7.843</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>2046</v>
+        <f aca="false">AVERAGE(B17:D17)</f>
+        <v>7.828</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>25</v>
+        <v>1027</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -475,9 +518,21 @@
         <v>1.029</v>
       </c>
       <c r="E18" s="0" t="n">
+        <f aca="false">AVERAGE(B18:D18)</f>
+        <v>0.993766666666667</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>2046</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="0" t="n">
         <v>9860</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="G19" s="0" t="n">
         <v>37</v>
       </c>
     </row>
@@ -514,10 +569,8 @@
         <v>9.496</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>821</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>31</v>
+        <f aca="false">AVERAGE(B22:D22)</f>
+        <v>9.46233333333333</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,10 +587,14 @@
         <v>2.048</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>2652</v>
+        <f aca="false">AVERAGE(B23:D23)</f>
+        <v>1.88033333333333</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>37</v>
+        <v>821</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,9 +611,21 @@
         <v>0.74</v>
       </c>
       <c r="E24" s="0" t="n">
+        <f aca="false">AVERAGE(B24:D24)</f>
+        <v>0.734066666666667</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>2652</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25" s="0" t="n">
         <v>10550</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="G25" s="0" t="n">
         <v>66</v>
       </c>
     </row>
@@ -592,11 +661,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1377551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,10 +1198,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,6 +1223,9 @@
       <c r="E2" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1441,7 +1509,7 @@
         <v>1.77166666666667</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1460,24 +1528,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:H9"/>
+  <dimension ref="A2:J9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -1489,15 +1555,18 @@
         <v>3</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4.12</v>
@@ -1514,16 +1583,20 @@
       <c r="F3" s="0" t="n">
         <v>3.725</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="0" t="n">
+      <c r="G3" s="0" t="n">
+        <f aca="false">AVERAGE(B3:F3)</f>
+        <v>3.8248</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="0" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3.85</v>
@@ -1540,10 +1613,14 @@
       <c r="F4" s="0" t="n">
         <v>3.856</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">AVERAGE(B4:F4)</f>
+        <v>3.8868</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1.369</v>
@@ -1560,30 +1637,34 @@
       <c r="F5" s="0" t="n">
         <v>1.428</v>
       </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">AVERAGE(B5:F5)</f>
+        <v>1.4044</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>43062</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>